<commit_message>
Update test fixtures to use sample from Ashish
</commit_message>
<xml_diff>
--- a/tests/fixtures/mel.xlsx
+++ b/tests/fixtures/mel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devan/Workspace/technogen/eloader/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devan/Workspace/technogen/eloader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815ACE10-B4B1-5C48-9A63-4D5E6CC7A93B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A62C392-813C-FB4B-9034-E167B0EFE71F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="0" windowWidth="31860" windowHeight="20580" xr2:uid="{2086CFB6-0ED6-514D-BC54-1F856B5652DB}"/>
+    <workbookView xWindow="1160" yWindow="1020" windowWidth="40780" windowHeight="20580" xr2:uid="{2086CFB6-0ED6-514D-BC54-1F856B5652DB}"/>
   </bookViews>
   <sheets>
     <sheet name="MEL" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MEL!$A$7:$N$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MEL!$A$7:$N$26</definedName>
     <definedName name="Alum_Data">#REF!</definedName>
     <definedName name="APPROVED_BY">[1]Info!$C$9</definedName>
     <definedName name="Breaker_Rated_Current">#REF!</definedName>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="71">
   <si>
     <t>Project:</t>
   </si>
@@ -187,15 +187,6 @@
     <t>FD</t>
   </si>
   <si>
-    <t>001 (A)</t>
-  </si>
-  <si>
-    <t>Compaction Feed Bucket Elevator</t>
-  </si>
-  <si>
-    <t>Switchroom 1</t>
-  </si>
-  <si>
     <t>DOL</t>
   </si>
   <si>
@@ -211,171 +202,143 @@
     <t>002</t>
   </si>
   <si>
-    <t>Compactor Feed Drag Conveyor</t>
-  </si>
-  <si>
-    <t>003 (A)</t>
-  </si>
-  <si>
-    <t>Metering Screw Conveyor</t>
-  </si>
-  <si>
-    <t>AA</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
-    <t>Compactor</t>
-  </si>
-  <si>
     <t>VSD</t>
   </si>
   <si>
-    <t>Force Feeders</t>
-  </si>
-  <si>
-    <t>Feeder</t>
-  </si>
-  <si>
-    <t>RB</t>
-  </si>
-  <si>
-    <t>Flake Breaker</t>
-  </si>
-  <si>
-    <t>004 (A)</t>
-  </si>
-  <si>
-    <t>Compactor Flake Drag Conveyor</t>
-  </si>
-  <si>
-    <t>Compaction Screen Bucket Elevator</t>
-  </si>
-  <si>
     <t>SN</t>
   </si>
   <si>
-    <t>Compaction Screen</t>
-  </si>
-  <si>
     <t>CR</t>
   </si>
   <si>
-    <t>Crusher</t>
-  </si>
-  <si>
-    <t>004</t>
-  </si>
-  <si>
-    <t>Crushed Flake Drag Conveyor</t>
-  </si>
-  <si>
     <t>005</t>
   </si>
   <si>
-    <t>Fines Recycle Drag Conveyor</t>
-  </si>
-  <si>
-    <t>Granular Product Belt Conveyor</t>
-  </si>
-  <si>
-    <t>AG</t>
-  </si>
-  <si>
-    <t>Granular Product Curing Drum</t>
-  </si>
-  <si>
-    <t>002 (A)</t>
-  </si>
-  <si>
-    <t>Reagent Screw Mixer</t>
-  </si>
-  <si>
     <t>PP</t>
   </si>
   <si>
-    <t>Dedusting Oil Pump</t>
-  </si>
-  <si>
     <t>012</t>
   </si>
   <si>
-    <t>Final Product Belt Conveyor</t>
-  </si>
-  <si>
-    <t>003</t>
-  </si>
-  <si>
-    <t>Compaction Area Dust Recycle Screw Conveyor</t>
-  </si>
-  <si>
     <t>010</t>
   </si>
   <si>
-    <t>Dust Recycle Drag Conveyor</t>
-  </si>
-  <si>
     <t>FN</t>
   </si>
   <si>
-    <t>Compaction Area Dust Recycle Fan</t>
-  </si>
-  <si>
-    <t>GA</t>
-  </si>
-  <si>
-    <t>Loadout Area Dust Recycle Rotary Valve</t>
-  </si>
-  <si>
     <t>011</t>
   </si>
   <si>
-    <t>Fines Bypass Drag Conveyor</t>
-  </si>
-  <si>
     <t>CP</t>
   </si>
   <si>
-    <t>001A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cooling  Skid </t>
-  </si>
-  <si>
-    <t>001B</t>
-  </si>
-  <si>
     <t>014</t>
   </si>
   <si>
-    <t>SSOP Transfer Belt Conveyor</t>
-  </si>
-  <si>
-    <t>015</t>
-  </si>
-  <si>
-    <t>WSSOP Product Belt Conveyor</t>
-  </si>
-  <si>
-    <t>Reagent Mixer</t>
-  </si>
-  <si>
-    <t>Switchroom 2</t>
-  </si>
-  <si>
-    <t>Loadout Area Dust Recycle Fan</t>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>DR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HP</t>
+  </si>
+  <si>
+    <t>LS</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIMARY CRUSHER JIB CRANE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIMARY CRUSHING AIR COMPRESSOR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIMARY CRUSHER </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIMARY FEEDER DRIBBLE CONVEYOR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIMARY CRUSHING AIR COMPRESSED AIR DRYER </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIMARY FEEDER MOTOR COOLING FAN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIMARY CRUSHER DUST COLLECTOR FAN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIMARY FEEDER </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIMARY CRUSHER WATER PUMP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIMARY VIBRATING GRIZZLY </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIMARY CRUSHER HYDRAULIC POWER PACK </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIMARY CRUSHER LUBRICATION UNIT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIMARY CRUSHING ROCK BREAKER HYDRAULIC POWERPACK1 </t>
+  </si>
+  <si>
+    <t>PRIMARY CRUSHING ROCK BREAKER HYDRAULIC POWERPACK2</t>
+  </si>
+  <si>
+    <t>PRIMARY CRUSHING ROCK BREAKER HYDRAULIC POWERPACK3</t>
+  </si>
+  <si>
+    <t>PRIMARY CRUSHING ROCK BREAKER HYDRAULIC POWERPACK4</t>
+  </si>
+  <si>
+    <t>PRIMARY CRUSHING ROCK BREAKER HYDRAULIC POWERPACK5</t>
+  </si>
+  <si>
+    <t>PRIMARY CRUSHING ROCK BREAKER HYDRAULIC POWERPACK6</t>
+  </si>
+  <si>
+    <t>PRIMARY CRUSHING ROCK BREAKER HYDRAULIC POWERPACK7</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>013</t>
+  </si>
+  <si>
+    <t>MCC-001</t>
+  </si>
+  <si>
+    <t>MCC-002</t>
+  </si>
+  <si>
+    <t>MCC-003</t>
+  </si>
+  <si>
+    <t>FEEDER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="14">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,22 +412,15 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="10"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Tahoma"/>
+      <sz val="8"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -801,27 +757,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="20" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="4" borderId="20" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="4" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="21" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
@@ -832,9 +787,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -853,61 +805,127 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="13" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -916,158 +934,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{650F131C-43B9-174B-95E7-AA6DFEB38416}"/>
-    <cellStyle name="Normal 2 19" xfId="4" xr:uid="{D249A9FB-DD2F-304F-ADF2-CA5BA6CE4EF5}"/>
-    <cellStyle name="Normal 4" xfId="2" xr:uid="{B0E1D282-3BA3-6740-AB99-EE1A2339D1E7}"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{650F131C-43B9-174B-95E7-AA6DFEB38416}"/>
+    <cellStyle name="Normal 2 19" xfId="3" xr:uid="{D249A9FB-DD2F-304F-ADF2-CA5BA6CE4EF5}"/>
+    <cellStyle name="Normal 4" xfId="1" xr:uid="{B0E1D282-3BA3-6740-AB99-EE1A2339D1E7}"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="21">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1296,7 +1173,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2874126</xdr:colOff>
+      <xdr:colOff>3119055</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>3539</xdr:rowOff>
     </xdr:to>
@@ -2801,15 +2678,15 @@
   <sheetPr codeName="Sheet19">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M42" sqref="M42"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9:L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="4.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="63.1640625" customWidth="1"/>
@@ -2823,144 +2700,144 @@
     <col min="15" max="15" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="38"/>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="47" t="str">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="28" t="str">
         <f>'[4]Standard Details'!E10</f>
         <v>POS4</v>
       </c>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="56" t="s">
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="57"/>
-      <c r="M1" s="58" t="str">
+      <c r="L1" s="38"/>
+      <c r="M1" s="39" t="str">
         <f>'[4]Standard Details'!E21</f>
         <v>Talison</v>
       </c>
-      <c r="N1" s="59"/>
+      <c r="N1" s="40"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="41"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="31" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="32"/>
-      <c r="M2" s="33" t="str">
+      <c r="L2" s="42"/>
+      <c r="M2" s="43" t="str">
         <f>'[4]Standard Details'!E22</f>
         <v>A</v>
       </c>
-      <c r="N2" s="30"/>
+      <c r="N2" s="44"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="16" thickBot="1">
-      <c r="A3" s="41"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="31" t="s">
+    <row r="3" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="32"/>
-      <c r="M3" s="33" t="str">
+      <c r="L3" s="42"/>
+      <c r="M3" s="43" t="str">
         <f>'[4]Standard Details'!E23</f>
         <v>AG</v>
       </c>
-      <c r="N3" s="30"/>
+      <c r="N3" s="44"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="41"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="60" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="22"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="31" t="s">
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="32"/>
-      <c r="M4" s="29">
+      <c r="L4" s="42"/>
+      <c r="M4" s="54">
         <f>'[4]Standard Details'!E24</f>
         <v>44099</v>
       </c>
-      <c r="N4" s="30"/>
+      <c r="N4" s="44"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="41"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="31" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="22"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="32"/>
-      <c r="M5" s="33" t="str">
+      <c r="L5" s="42"/>
+      <c r="M5" s="43" t="str">
         <f>'[4]Standard Details'!E25</f>
         <v>RN</v>
       </c>
-      <c r="N5" s="30"/>
+      <c r="N5" s="44"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" ht="16" thickBot="1">
-      <c r="A6" s="44"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="67"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="34" t="s">
+    <row r="6" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="25"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="35"/>
-      <c r="M6" s="36">
+      <c r="L6" s="56"/>
+      <c r="M6" s="57">
         <f>'[4]Standard Details'!E26</f>
         <v>44099</v>
       </c>
-      <c r="N6" s="37"/>
+      <c r="N6" s="58"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15" ht="29" thickBot="1">
+    <row r="7" spans="1:15" ht="29" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -3005,1404 +2882,954 @@
       </c>
       <c r="O7" s="7"/>
     </row>
-    <row r="8" spans="1:15" ht="22.5" customHeight="1">
+    <row r="8" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
-        <v>3100</v>
+        <v>121</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="C8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="59" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="9">
+        <v>2</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="12">
+        <v>20</v>
+      </c>
+      <c r="H8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="I8" s="13">
+        <v>415</v>
+      </c>
+      <c r="J8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="9">
+      <c r="K8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="15">
         <v>5</v>
       </c>
-      <c r="F8" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="13">
-        <v>14.914020670832649</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="14">
-        <v>415</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L8" s="16">
-        <v>4</v>
-      </c>
-      <c r="M8" s="17" t="str">
+      <c r="M8" s="16" t="str">
         <f>IF(L8="","",VLOOKUP(L8,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N8" s="18" t="str">
+        <v>Final Certified Vendor Data (AS BUILT)</v>
+      </c>
+      <c r="N8" s="17" t="str">
         <f>A8&amp;B8&amp;C8</f>
-        <v>3100FD001 (A)</v>
+        <v>121CN001</v>
       </c>
       <c r="O8" s="8" t="str">
         <f>VLOOKUP(B8,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>FD</v>
+        <v>CN</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="22.5" customHeight="1">
+    <row r="9" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
-        <v>3100</v>
+        <v>121</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="D9" s="59" t="s">
+        <v>45</v>
       </c>
       <c r="E9" s="9">
+        <v>2</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="12">
+        <v>7.5</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" s="13">
+        <v>415</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" s="15">
         <v>5</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="13">
-        <v>7.4570103354163244</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="14">
-        <v>415</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L9" s="16">
-        <v>4</v>
-      </c>
-      <c r="M9" s="17" t="str">
+      <c r="M9" s="16" t="str">
         <f>IF(L9="","",VLOOKUP(L9,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N9" s="18" t="str">
-        <f t="shared" ref="N9:N35" si="0">A9&amp;B9&amp;C9</f>
-        <v>3100CV002</v>
+        <v>Final Certified Vendor Data (AS BUILT)</v>
+      </c>
+      <c r="N9" s="17" t="str">
+        <f t="shared" ref="N9:N26" si="0">A9&amp;B9&amp;C9</f>
+        <v>121CP001</v>
       </c>
       <c r="O9" s="8" t="str">
         <f>VLOOKUP(B9,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>CV</v>
+        <v>CP</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="22.5" customHeight="1">
+    <row r="10" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
-        <v>3100</v>
+        <v>121</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="9">
+        <v>2</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" s="12">
+        <v>10</v>
+      </c>
+      <c r="H10" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="9">
+      <c r="I10" s="13">
+        <v>415</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" s="15">
         <v>5</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="13">
-        <v>7.4570103354163244</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="14">
-        <v>415</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K10" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L10" s="16">
-        <v>4</v>
-      </c>
-      <c r="M10" s="17" t="str">
+      <c r="M10" s="16" t="str">
         <f>IF(L10="","",VLOOKUP(L10,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N10" s="18" t="str">
+        <v>Final Certified Vendor Data (AS BUILT)</v>
+      </c>
+      <c r="N10" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>3100CV003 (A)</v>
+        <v>121CR001</v>
       </c>
       <c r="O10" s="8" t="str">
         <f>VLOOKUP(B10,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>CV</v>
+        <v>CR</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="22.5" customHeight="1">
+    <row r="11" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
-        <v>3100</v>
+        <v>121</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="D11" s="59" t="s">
+        <v>47</v>
       </c>
       <c r="E11" s="9">
-        <v>6</v>
-      </c>
-      <c r="F11" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="11">
+        <v>415</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="13">
-        <v>745.70103354163246</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="I11" s="12">
-        <v>415</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L11" s="16">
-        <v>4</v>
-      </c>
-      <c r="M11" s="17" t="str">
+      <c r="L11" s="15">
+        <v>5</v>
+      </c>
+      <c r="M11" s="16" t="str">
         <f>IF(L11="","",VLOOKUP(L11,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N11" s="18" t="str">
+        <v>Final Certified Vendor Data (AS BUILT)</v>
+      </c>
+      <c r="N11" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>3100AA001</v>
+        <v>121CV005</v>
       </c>
       <c r="O11" s="8" t="str">
         <f>VLOOKUP(B11,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>AA</v>
+        <v>CV</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="22.5" customHeight="1">
+    <row r="12" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
-        <v>3100</v>
+        <v>121</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>37</v>
+        <v>27</v>
+      </c>
+      <c r="D12" s="59" t="s">
+        <v>48</v>
       </c>
       <c r="E12" s="9">
-        <v>6</v>
-      </c>
-      <c r="F12" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="11">
+        <v>415</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="13">
-        <v>111.85515503124486</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="12">
-        <v>415</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L12" s="16">
-        <v>4</v>
-      </c>
-      <c r="M12" s="17" t="str">
+      <c r="L12" s="15">
+        <v>5</v>
+      </c>
+      <c r="M12" s="16" t="str">
         <f>IF(L12="","",VLOOKUP(L12,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N12" s="18" t="str">
+        <v>Final Certified Vendor Data (AS BUILT)</v>
+      </c>
+      <c r="N12" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>3100FD001</v>
+        <v>121DR001</v>
       </c>
       <c r="O12" s="8" t="str">
         <f>VLOOKUP(B12,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>FD</v>
+        <v>DR</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
-        <v>3100</v>
+        <v>121</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>40</v>
+        <v>27</v>
+      </c>
+      <c r="D13" s="59" t="s">
+        <v>49</v>
       </c>
       <c r="E13" s="9">
-        <v>6</v>
-      </c>
-      <c r="F13" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="13">
+        <v>415</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="13">
-        <v>22.371031006248973</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13" s="14">
-        <v>415</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L13" s="16">
-        <v>4</v>
-      </c>
-      <c r="M13" s="17" t="str">
+      <c r="L13" s="15">
+        <v>5</v>
+      </c>
+      <c r="M13" s="16" t="str">
         <f>IF(L13="","",VLOOKUP(L13,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N13" s="18" t="str">
+        <v>Final Certified Vendor Data (AS BUILT)</v>
+      </c>
+      <c r="N13" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>3100RB001</v>
+        <v>121FN001</v>
       </c>
       <c r="O13" s="8" t="str">
         <f>VLOOKUP(B13,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>RB</v>
+        <v>FN</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="28">
+    <row r="14" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
-        <v>3100</v>
+        <v>121</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>42</v>
+        <v>26</v>
+      </c>
+      <c r="D14" s="59" t="s">
+        <v>50</v>
       </c>
       <c r="E14" s="9">
-        <v>6</v>
-      </c>
-      <c r="F14" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="12">
+        <v>3</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="13">
+        <v>415</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="13">
-        <v>7.4570103354163244</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14" s="14">
-        <v>415</v>
-      </c>
-      <c r="J14" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L14" s="16">
-        <v>4</v>
-      </c>
-      <c r="M14" s="17" t="str">
+      <c r="L14" s="15">
+        <v>5</v>
+      </c>
+      <c r="M14" s="16" t="str">
         <f>IF(L14="","",VLOOKUP(L14,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N14" s="18" t="str">
+        <v>Final Certified Vendor Data (AS BUILT)</v>
+      </c>
+      <c r="N14" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>3100CV004 (A)</v>
+        <v>121FN002</v>
       </c>
       <c r="O14" s="8" t="str">
         <f>VLOOKUP(B14,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>CV</v>
+        <v>FN</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
-        <v>3100</v>
+        <v>121</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>43</v>
+        <v>27</v>
+      </c>
+      <c r="D15" s="59" t="s">
+        <v>51</v>
       </c>
       <c r="E15" s="9">
+        <v>2</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="12">
+        <v>55</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I15" s="13">
+        <v>415</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L15" s="15">
         <v>5</v>
       </c>
-      <c r="F15" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="13">
-        <v>29.828041341665298</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I15" s="14">
-        <v>415</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K15" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L15" s="16">
-        <v>4</v>
-      </c>
-      <c r="M15" s="17" t="str">
+      <c r="M15" s="16" t="str">
         <f>IF(L15="","",VLOOKUP(L15,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N15" s="18" t="str">
+        <v>Final Certified Vendor Data (AS BUILT)</v>
+      </c>
+      <c r="N15" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>3100FD002</v>
+        <v>121FD001</v>
       </c>
       <c r="O15" s="8" t="str">
         <f>VLOOKUP(B15,[4]Database!$U$3:$V$39,1,FALSE)</f>
         <v>FD</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
-        <v>3100</v>
+        <v>121</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>45</v>
+        <v>27</v>
+      </c>
+      <c r="D16" s="59" t="s">
+        <v>52</v>
       </c>
       <c r="E16" s="9">
+        <v>2</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="12">
+        <v>4</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I16" s="13">
+        <v>415</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L16" s="15">
         <v>5</v>
       </c>
-      <c r="F16" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="13">
-        <v>14.914020670832649</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I16" s="14">
-        <v>415</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K16" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L16" s="16">
-        <v>4</v>
-      </c>
-      <c r="M16" s="17" t="str">
+      <c r="M16" s="16" t="str">
         <f>IF(L16="","",VLOOKUP(L16,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N16" s="18" t="str">
+        <v>Final Certified Vendor Data (AS BUILT)</v>
+      </c>
+      <c r="N16" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>3100SN001</v>
+        <v>121PP001</v>
       </c>
       <c r="O16" s="8" t="str">
         <f>VLOOKUP(B16,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>SN</v>
+        <v>PP</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
-        <v>3100</v>
+        <v>121</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>47</v>
+        <v>27</v>
+      </c>
+      <c r="D17" s="59" t="s">
+        <v>53</v>
       </c>
       <c r="E17" s="9">
+        <v>2</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="12">
+        <v>37</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="11">
+        <v>415</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L17" s="15">
         <v>5</v>
       </c>
-      <c r="F17" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" s="13">
-        <v>149.14020670832647</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="I17" s="12">
-        <v>415</v>
-      </c>
-      <c r="J17" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K17" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L17" s="16">
-        <v>4</v>
-      </c>
-      <c r="M17" s="17" t="str">
+      <c r="M17" s="16" t="str">
         <f>IF(L17="","",VLOOKUP(L17,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N17" s="18" t="str">
+        <v>Final Certified Vendor Data (AS BUILT)</v>
+      </c>
+      <c r="N17" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>3100CR001</v>
+        <v>121SN001</v>
       </c>
       <c r="O17" s="8" t="str">
         <f>VLOOKUP(B17,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>CR</v>
+        <v>SN</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
-        <v>3100</v>
+        <v>121</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>49</v>
+        <v>31</v>
+      </c>
+      <c r="D18" s="59" t="s">
+        <v>54</v>
       </c>
       <c r="E18" s="9">
+        <v>2</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" s="18">
+        <v>3.7</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I18" s="13">
+        <v>415</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L18" s="15">
         <v>5</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="M18" s="16" t="str">
+        <f>IF(L18="","",VLOOKUP(L18,[4]Database!$N$49:$P$53,3,FALSE))</f>
+        <v>Final Certified Vendor Data (AS BUILT)</v>
+      </c>
+      <c r="N18" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>121 HP005</v>
+      </c>
+      <c r="O18" s="8" t="e">
+        <f>VLOOKUP(B18,[4]Database!$U$3:$V$39,1,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="8">
+        <v>121</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="59" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="9">
+        <v>2</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I19" s="13">
+        <v>415</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="20">
+      <c r="L19" s="15">
         <v>5</v>
       </c>
-      <c r="H18" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" s="14">
-        <v>415</v>
-      </c>
-      <c r="J18" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K18" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L18" s="16">
-        <v>4</v>
-      </c>
-      <c r="M18" s="17" t="str">
-        <f>IF(L18="","",VLOOKUP(L18,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N18" s="18" t="str">
+      <c r="M19" s="16" t="str">
+        <f>IF(L19="","",VLOOKUP(L19,[4]Database!$N$49:$P$53,3,FALSE))</f>
+        <v>Final Certified Vendor Data (AS BUILT)</v>
+      </c>
+      <c r="N19" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>3100CV004</v>
-      </c>
-      <c r="O18" s="8" t="str">
-        <f>VLOOKUP(B18,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>CV</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
-      <c r="A19" s="8">
-        <v>3100</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" s="9">
-        <v>5</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" s="13">
-        <v>7.4570103354163244</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19" s="14">
-        <v>415</v>
-      </c>
-      <c r="J19" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K19" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L19" s="16">
-        <v>4</v>
-      </c>
-      <c r="M19" s="17" t="str">
-        <f>IF(L19="","",VLOOKUP(L19,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N19" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>3100CV005</v>
+        <v>121LS006</v>
       </c>
       <c r="O19" s="8" t="str">
         <f>VLOOKUP(B19,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>CV</v>
+        <v>LS</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
-        <v>3100</v>
+        <v>121</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>52</v>
+        <v>64</v>
+      </c>
+      <c r="D20" s="59" t="s">
+        <v>56</v>
       </c>
       <c r="E20" s="9">
-        <v>4</v>
-      </c>
-      <c r="F20" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" s="18">
+        <v>37</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I20" s="13">
+        <v>415</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="20">
+      <c r="L20" s="15">
         <v>5</v>
       </c>
-      <c r="H20" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I20" s="14">
-        <v>415</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K20" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L20" s="16">
-        <v>4</v>
-      </c>
-      <c r="M20" s="17" t="str">
+      <c r="M20" s="16" t="str">
         <f>IF(L20="","",VLOOKUP(L20,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N20" s="18" t="str">
+        <v>Final Certified Vendor Data (AS BUILT)</v>
+      </c>
+      <c r="N20" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>3100CV001</v>
+        <v>121HP008</v>
       </c>
       <c r="O20" s="8" t="str">
         <f>VLOOKUP(B20,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>CV</v>
+        <v>HP</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
-        <v>3100</v>
+        <v>121</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>54</v>
+        <v>65</v>
+      </c>
+      <c r="D21" s="59" t="s">
+        <v>57</v>
       </c>
       <c r="E21" s="9">
-        <v>4</v>
-      </c>
-      <c r="F21" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" s="18">
+        <v>37</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I21" s="13">
+        <v>415</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="13">
-        <v>11.185515503124487</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I21" s="14">
-        <v>415</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K21" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L21" s="16">
-        <v>4</v>
-      </c>
-      <c r="M21" s="17" t="str">
+      <c r="L21" s="15">
+        <v>5</v>
+      </c>
+      <c r="M21" s="16" t="str">
         <f>IF(L21="","",VLOOKUP(L21,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N21" s="18" t="str">
+        <v>Final Certified Vendor Data (AS BUILT)</v>
+      </c>
+      <c r="N21" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>3100AG001</v>
+        <v>121HP009</v>
       </c>
       <c r="O21" s="8" t="str">
         <f>VLOOKUP(B21,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>AG</v>
+        <v>HP</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="28">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
-        <v>3100</v>
+        <v>121</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>56</v>
+        <v>34</v>
+      </c>
+      <c r="D22" s="59" t="s">
+        <v>58</v>
       </c>
       <c r="E22" s="9">
-        <v>4</v>
-      </c>
-      <c r="F22" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G22" s="18">
+        <v>37</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I22" s="13">
+        <v>415</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G22" s="13">
-        <v>7.4570103354163244</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I22" s="14">
-        <v>415</v>
-      </c>
-      <c r="J22" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K22" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L22" s="16">
-        <v>4</v>
-      </c>
-      <c r="M22" s="17" t="str">
+      <c r="L22" s="15">
+        <v>5</v>
+      </c>
+      <c r="M22" s="16" t="str">
         <f>IF(L22="","",VLOOKUP(L22,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N22" s="18" t="str">
+        <v>Final Certified Vendor Data (AS BUILT)</v>
+      </c>
+      <c r="N22" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>3100AG002 (A)</v>
+        <v>121HP010</v>
       </c>
       <c r="O22" s="8" t="str">
         <f>VLOOKUP(B22,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>AG</v>
+        <v>HP</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
-        <v>3100</v>
+        <v>121</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>58</v>
+        <v>36</v>
+      </c>
+      <c r="D23" s="59" t="s">
+        <v>59</v>
       </c>
       <c r="E23" s="9">
+        <v>2</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" s="18">
+        <v>37</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I23" s="13">
+        <v>415</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L23" s="15">
         <v>5</v>
       </c>
-      <c r="F23" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G23" s="22">
-        <v>3.7285051677081622</v>
-      </c>
-      <c r="H23" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I23" s="14">
-        <v>415</v>
-      </c>
-      <c r="J23" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K23" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L23" s="16">
-        <v>4</v>
-      </c>
-      <c r="M23" s="17" t="str">
+      <c r="M23" s="16" t="str">
         <f>IF(L23="","",VLOOKUP(L23,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N23" s="18" t="str">
+        <v>Final Certified Vendor Data (AS BUILT)</v>
+      </c>
+      <c r="N23" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>3100PP001</v>
+        <v>121HP011</v>
       </c>
       <c r="O23" s="8" t="str">
         <f>VLOOKUP(B23,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>PP</v>
+        <v>HP</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
-        <v>3100</v>
+        <v>121</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="59" t="s">
         <v>60</v>
       </c>
       <c r="E24" s="9">
+        <v>2</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="18">
+        <v>37</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I24" s="13">
+        <v>415</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L24" s="15">
         <v>5</v>
       </c>
-      <c r="F24" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24" s="22">
-        <v>14.914020670832649</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I24" s="14">
-        <v>415</v>
-      </c>
-      <c r="J24" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K24" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L24" s="16">
-        <v>4</v>
-      </c>
-      <c r="M24" s="17" t="str">
+      <c r="M24" s="16" t="str">
         <f>IF(L24="","",VLOOKUP(L24,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N24" s="18" t="str">
+        <v>Final Certified Vendor Data (AS BUILT)</v>
+      </c>
+      <c r="N24" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>3100CV012</v>
+        <v>121HP012</v>
       </c>
       <c r="O24" s="8" t="str">
         <f>VLOOKUP(B24,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>CV</v>
+        <v>HP</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
-      <c r="A25" s="23">
-        <v>3100</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="24" t="s">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="8">
+        <v>121</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="19" t="s">
-        <v>62</v>
-      </c>
       <c r="E25" s="9">
+        <v>2</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="18">
+        <v>37</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I25" s="13">
+        <v>415</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L25" s="15">
         <v>5</v>
       </c>
-      <c r="F25" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G25" s="13">
-        <v>5.5927577515622433</v>
-      </c>
-      <c r="H25" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I25" s="14">
-        <v>415</v>
-      </c>
-      <c r="J25" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K25" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L25" s="16">
-        <v>4</v>
-      </c>
-      <c r="M25" s="17" t="str">
+      <c r="M25" s="16" t="str">
         <f>IF(L25="","",VLOOKUP(L25,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N25" s="18" t="str">
+        <v>Final Certified Vendor Data (AS BUILT)</v>
+      </c>
+      <c r="N25" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>3100CV003</v>
+        <v>121HP013</v>
       </c>
       <c r="O25" s="8" t="str">
         <f>VLOOKUP(B25,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>CV</v>
+        <v>HP</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
-      <c r="A26" s="23">
-        <v>3100</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>28</v>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="8">
+        <v>121</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>64</v>
+        <v>38</v>
+      </c>
+      <c r="D26" s="59" t="s">
+        <v>62</v>
       </c>
       <c r="E26" s="9">
+        <v>2</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" s="18">
+        <v>37</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I26" s="13">
+        <v>415</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L26" s="15">
         <v>5</v>
       </c>
-      <c r="F26" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" s="20">
-        <v>5</v>
-      </c>
-      <c r="H26" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I26" s="14">
-        <v>415</v>
-      </c>
-      <c r="J26" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K26" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L26" s="16">
-        <v>4</v>
-      </c>
-      <c r="M26" s="17" t="str">
+      <c r="M26" s="16" t="str">
         <f>IF(L26="","",VLOOKUP(L26,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N26" s="18" t="str">
+        <v>Final Certified Vendor Data (AS BUILT)</v>
+      </c>
+      <c r="N26" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>3100CV010</v>
+        <v>121HP014</v>
       </c>
       <c r="O26" s="8" t="str">
         <f>VLOOKUP(B26,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>CV</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15">
-      <c r="A27" s="23">
-        <v>3100</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="E27" s="9">
-        <v>5</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G27" s="13">
-        <v>29.828041341665298</v>
-      </c>
-      <c r="H27" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I27" s="14">
-        <v>415</v>
-      </c>
-      <c r="J27" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K27" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L27" s="16">
-        <v>4</v>
-      </c>
-      <c r="M27" s="17" t="str">
-        <f>IF(L27="","",VLOOKUP(L27,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N27" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>3100FN001</v>
-      </c>
-      <c r="O27" s="8" t="str">
-        <f>VLOOKUP(B27,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>FN</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15">
-      <c r="A28" s="23">
-        <v>3100</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="E28" s="9">
-        <v>5</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G28" s="13">
-        <v>1.1185515503124486</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I28" s="14">
-        <v>415</v>
-      </c>
-      <c r="J28" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K28" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L28" s="16">
-        <v>4</v>
-      </c>
-      <c r="M28" s="17" t="str">
-        <f>IF(L28="","",VLOOKUP(L28,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N28" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>3100GA002</v>
-      </c>
-      <c r="O28" s="8" t="str">
-        <f>VLOOKUP(B28,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>GA</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15">
-      <c r="A29" s="23">
-        <v>3100</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="D29" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" s="9">
-        <v>5</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G29" s="13">
-        <v>11.2</v>
-      </c>
-      <c r="H29" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I29" s="14">
-        <v>415</v>
-      </c>
-      <c r="J29" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K29" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L29" s="16">
-        <v>4</v>
-      </c>
-      <c r="M29" s="17" t="str">
-        <f>IF(L29="","",VLOOKUP(L29,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N29" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>3100CV011</v>
-      </c>
-      <c r="O29" s="8" t="str">
-        <f>VLOOKUP(B29,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>CV</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="28">
-      <c r="A30" s="23">
-        <v>3100</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E30" s="9">
-        <v>5</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G30" s="13">
-        <v>95</v>
-      </c>
-      <c r="H30" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I30" s="12">
-        <v>415</v>
-      </c>
-      <c r="J30" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K30" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L30" s="16">
-        <v>4</v>
-      </c>
-      <c r="M30" s="17" t="str">
-        <f>IF(L30="","",VLOOKUP(L30,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N30" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>3100CP001A</v>
-      </c>
-      <c r="O30" s="8" t="str">
-        <f>VLOOKUP(B30,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>CP</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="28">
-      <c r="A31" s="23">
-        <v>3100</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C31" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E31" s="9">
-        <v>5</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G31" s="13">
-        <v>30</v>
-      </c>
-      <c r="H31" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I31" s="14">
-        <v>415</v>
-      </c>
-      <c r="J31" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K31" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L31" s="16">
-        <v>4</v>
-      </c>
-      <c r="M31" s="17" t="str">
-        <f>IF(L31="","",VLOOKUP(L31,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N31" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>3100CP001B</v>
-      </c>
-      <c r="O31" s="8" t="str">
-        <f>VLOOKUP(B31,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>CP</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15">
-      <c r="A32" s="23">
-        <v>3100</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="E32" s="9">
-        <v>6</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G32" s="26">
-        <v>14.914020670832649</v>
-      </c>
-      <c r="H32" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I32" s="14">
-        <v>415</v>
-      </c>
-      <c r="J32" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K32" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L32" s="16">
-        <v>4</v>
-      </c>
-      <c r="M32" s="17" t="str">
-        <f>IF(L32="","",VLOOKUP(L32,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N32" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>3100CV014</v>
-      </c>
-      <c r="O32" s="8" t="str">
-        <f>VLOOKUP(B32,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>CV</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15">
-      <c r="A33" s="23">
-        <v>3100</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D33" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="E33" s="9">
-        <v>5</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G33" s="27">
-        <v>14.914020670832649</v>
-      </c>
-      <c r="H33" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I33" s="14">
-        <v>415</v>
-      </c>
-      <c r="J33" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K33" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L33" s="16">
-        <v>4</v>
-      </c>
-      <c r="M33" s="17" t="str">
-        <f>IF(L33="","",VLOOKUP(L33,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N33" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>3100CV015</v>
-      </c>
-      <c r="O33" s="8" t="str">
-        <f>VLOOKUP(B33,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>CV</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15">
-      <c r="A34" s="23">
-        <v>3100</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C34" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="E34" s="9">
-        <v>5</v>
-      </c>
-      <c r="F34" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="G34" s="13">
-        <v>29.8</v>
-      </c>
-      <c r="H34" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I34" s="14">
-        <v>415</v>
-      </c>
-      <c r="J34" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K34" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L34" s="16">
-        <v>4</v>
-      </c>
-      <c r="M34" s="17" t="str">
-        <f>IF(L34="","",VLOOKUP(L34,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N34" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>3100AG002</v>
-      </c>
-      <c r="O34" s="8" t="str">
-        <f>VLOOKUP(B34,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>AG</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15">
-      <c r="A35" s="23">
-        <v>3100</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="D35" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="E35" s="9">
-        <v>5</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="G35" s="28">
-        <v>29.8</v>
-      </c>
-      <c r="H35" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I35" s="14">
-        <v>415</v>
-      </c>
-      <c r="J35" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K35" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L35" s="16">
-        <v>4</v>
-      </c>
-      <c r="M35" s="17" t="str">
-        <f>IF(L35="","",VLOOKUP(L35,[4]Database!$N$49:$P$53,3,FALSE))</f>
-        <v>Prelim Post Award Data</v>
-      </c>
-      <c r="N35" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>3100FN011</v>
-      </c>
-      <c r="O35" s="8" t="str">
-        <f>VLOOKUP(B35,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>FN</v>
+        <v>HP</v>
       </c>
     </row>
   </sheetData>
@@ -4424,87 +3851,31 @@
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="M6:N6"/>
   </mergeCells>
+  <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="D7">
-    <cfRule type="duplicateValues" dxfId="25" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7">
-    <cfRule type="duplicateValues" dxfId="24" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7">
-    <cfRule type="duplicateValues" dxfId="23" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N7">
-    <cfRule type="duplicateValues" dxfId="22" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="23"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M8:N35">
-    <cfRule type="expression" dxfId="21" priority="22">
+  <conditionalFormatting sqref="M8:N26">
+    <cfRule type="expression" dxfId="16" priority="22">
       <formula>ISERROR($O8)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M8:O35">
-    <cfRule type="expression" dxfId="20" priority="21">
+  <conditionalFormatting sqref="M8:O26">
+    <cfRule type="expression" dxfId="15" priority="21">
       <formula>ISNA($O8)=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11:D12">
-    <cfRule type="duplicateValues" dxfId="19" priority="20"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D21">
-    <cfRule type="duplicateValues" dxfId="18" priority="19"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D22">
-    <cfRule type="duplicateValues" dxfId="17" priority="18"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D20">
-    <cfRule type="duplicateValues" dxfId="16" priority="17"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D28 D26">
-    <cfRule type="duplicateValues" dxfId="15" priority="16"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D29">
-    <cfRule type="duplicateValues" dxfId="14" priority="15"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27">
-    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D25">
-    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D31:D33">
-    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30 D8:D10 D13">
-    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D19">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D23:D24">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N8:N35">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="N8:N26">
+    <cfRule type="duplicateValues" dxfId="0" priority="32"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added first of database tables.
</commit_message>
<xml_diff>
--- a/tests/fixtures/mel.xlsx
+++ b/tests/fixtures/mel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devan/Workspace/technogen/eloader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A62C392-813C-FB4B-9034-E167B0EFE71F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A594B5-CDE8-214F-8328-B735971B268A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1020" windowWidth="40780" windowHeight="20580" xr2:uid="{2086CFB6-0ED6-514D-BC54-1F856B5652DB}"/>
+    <workbookView xWindow="5380" yWindow="1140" windowWidth="38400" windowHeight="20580" xr2:uid="{2086CFB6-0ED6-514D-BC54-1F856B5652DB}"/>
   </bookViews>
   <sheets>
     <sheet name="MEL" sheetId="1" r:id="rId1"/>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="70">
   <si>
     <t>Project:</t>
   </si>
@@ -242,9 +242,6 @@
   </si>
   <si>
     <t>DR</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> HP</t>
   </si>
   <si>
     <t>LS</t>
@@ -814,6 +811,9 @@
     <xf numFmtId="4" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -932,9 +932,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -944,147 +941,7 @@
     <cellStyle name="Normal 2 19" xfId="3" xr:uid="{D249A9FB-DD2F-304F-ADF2-CA5BA6CE4EF5}"/>
     <cellStyle name="Normal 4" xfId="1" xr:uid="{B0E1D282-3BA3-6740-AB99-EE1A2339D1E7}"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1997,7 +1854,7 @@
         </row>
         <row r="24">
           <cell r="E24">
-            <v>44099</v>
+            <v>44110</v>
           </cell>
         </row>
         <row r="25">
@@ -2007,7 +1864,7 @@
         </row>
         <row r="26">
           <cell r="E26">
-            <v>44099</v>
+            <v>44110</v>
           </cell>
         </row>
       </sheetData>
@@ -2680,8 +2537,8 @@
   </sheetPr>
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9:L26"/>
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2701,140 +2558,140 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="19"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="28" t="str">
+      <c r="A1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="29" t="str">
         <f>'[4]Standard Details'!E10</f>
         <v>POS4</v>
       </c>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="37" t="s">
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="38"/>
-      <c r="M1" s="39" t="str">
+      <c r="L1" s="39"/>
+      <c r="M1" s="40" t="str">
         <f>'[4]Standard Details'!E21</f>
         <v>Talison</v>
       </c>
-      <c r="N1" s="40"/>
+      <c r="N1" s="41"/>
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="41" t="s">
+      <c r="A2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="42"/>
-      <c r="M2" s="43" t="str">
+      <c r="L2" s="43"/>
+      <c r="M2" s="44" t="str">
         <f>'[4]Standard Details'!E22</f>
         <v>A</v>
       </c>
-      <c r="N2" s="44"/>
+      <c r="N2" s="45"/>
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="41" t="s">
+      <c r="A3" s="23"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="42"/>
-      <c r="M3" s="43" t="str">
+      <c r="L3" s="43"/>
+      <c r="M3" s="44" t="str">
         <f>'[4]Standard Details'!E23</f>
         <v>AG</v>
       </c>
-      <c r="N3" s="44"/>
+      <c r="N3" s="45"/>
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="22"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="45" t="s">
+      <c r="A4" s="23"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="41" t="s">
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="42"/>
-      <c r="M4" s="54">
-        <f>'[4]Standard Details'!E24</f>
-        <v>44099</v>
-      </c>
-      <c r="N4" s="44"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="55">
+        <f ca="1">'[4]Standard Details'!E24</f>
+        <v>44110</v>
+      </c>
+      <c r="N4" s="45"/>
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="22"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="41" t="s">
+      <c r="A5" s="23"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="42"/>
-      <c r="M5" s="43" t="str">
+      <c r="L5" s="43"/>
+      <c r="M5" s="44" t="str">
         <f>'[4]Standard Details'!E25</f>
         <v>RN</v>
       </c>
-      <c r="N5" s="44"/>
+      <c r="N5" s="45"/>
       <c r="O5" s="1"/>
     </row>
     <row r="6" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="55" t="s">
+      <c r="A6" s="26"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="56"/>
-      <c r="M6" s="57">
-        <f>'[4]Standard Details'!E26</f>
-        <v>44099</v>
-      </c>
-      <c r="N6" s="58"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="58">
+        <f ca="1">'[4]Standard Details'!E26</f>
+        <v>44110</v>
+      </c>
+      <c r="N6" s="59"/>
       <c r="O6" s="2"/>
     </row>
     <row r="7" spans="1:15" ht="29" thickBot="1" x14ac:dyDescent="0.25">
@@ -2892,14 +2749,14 @@
       <c r="C8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="59" t="s">
-        <v>44</v>
+      <c r="D8" s="19" t="s">
+        <v>43</v>
       </c>
       <c r="E8" s="9">
         <v>2</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G8" s="12">
         <v>20</v>
@@ -2942,20 +2799,20 @@
       <c r="C9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="59" t="s">
-        <v>45</v>
+      <c r="D9" s="19" t="s">
+        <v>44</v>
       </c>
       <c r="E9" s="9">
         <v>2</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G9" s="12">
         <v>7.5</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I9" s="13">
         <v>415</v>
@@ -2992,14 +2849,14 @@
       <c r="C10" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="59" t="s">
-        <v>46</v>
+      <c r="D10" s="19" t="s">
+        <v>45</v>
       </c>
       <c r="E10" s="9">
         <v>2</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G10" s="12">
         <v>10</v>
@@ -3042,14 +2899,14 @@
       <c r="C11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="59" t="s">
-        <v>47</v>
+      <c r="D11" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="E11" s="9">
         <v>2</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G11" s="12">
         <v>2.2000000000000002</v>
@@ -3092,14 +2949,14 @@
       <c r="C12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="59" t="s">
-        <v>48</v>
+      <c r="D12" s="19" t="s">
+        <v>47</v>
       </c>
       <c r="E12" s="9">
         <v>2</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G12" s="12">
         <v>0.1</v>
@@ -3132,7 +2989,7 @@
         <v>DR</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="28" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>121</v>
       </c>
@@ -3142,14 +2999,14 @@
       <c r="C13" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="59" t="s">
-        <v>49</v>
+      <c r="D13" s="19" t="s">
+        <v>48</v>
       </c>
       <c r="E13" s="9">
         <v>2</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G13" s="12">
         <v>0.2</v>
@@ -3192,14 +3049,14 @@
       <c r="C14" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="59" t="s">
-        <v>50</v>
+      <c r="D14" s="19" t="s">
+        <v>49</v>
       </c>
       <c r="E14" s="9">
         <v>2</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G14" s="12">
         <v>3</v>
@@ -3232,7 +3089,7 @@
         <v>FN</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="28" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>121</v>
       </c>
@@ -3242,20 +3099,20 @@
       <c r="C15" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="59" t="s">
-        <v>51</v>
+      <c r="D15" s="19" t="s">
+        <v>50</v>
       </c>
       <c r="E15" s="9">
         <v>2</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G15" s="12">
         <v>55</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I15" s="13">
         <v>415</v>
@@ -3282,7 +3139,7 @@
         <v>FD</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="28" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>121</v>
       </c>
@@ -3292,20 +3149,20 @@
       <c r="C16" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="59" t="s">
-        <v>52</v>
+      <c r="D16" s="19" t="s">
+        <v>51</v>
       </c>
       <c r="E16" s="9">
         <v>2</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G16" s="12">
         <v>4</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I16" s="13">
         <v>415</v>
@@ -3332,7 +3189,7 @@
         <v>PP</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="28" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <v>121</v>
       </c>
@@ -3342,14 +3199,14 @@
       <c r="C17" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="59" t="s">
-        <v>53</v>
+      <c r="D17" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="E17" s="9">
         <v>2</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G17" s="12">
         <v>37</v>
@@ -3382,30 +3239,30 @@
         <v>SN</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="28" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>121</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="59" t="s">
-        <v>54</v>
+      <c r="D18" s="19" t="s">
+        <v>53</v>
       </c>
       <c r="E18" s="9">
         <v>2</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G18" s="18">
         <v>3.7</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I18" s="13">
         <v>415</v>
@@ -3424,38 +3281,38 @@
         <v>Final Certified Vendor Data (AS BUILT)</v>
       </c>
       <c r="N18" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>121 HP005</v>
-      </c>
-      <c r="O18" s="8" t="e">
+        <f t="shared" ref="N18" si="1">A18&amp;B18&amp;C18</f>
+        <v>121HP005</v>
+      </c>
+      <c r="O18" s="8" t="str">
         <f>VLOOKUP(B18,[4]Database!$U$3:$V$39,1,FALSE)</f>
-        <v>#N/A</v>
+        <v>HP</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="28" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>121</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="59" t="s">
-        <v>55</v>
+        <v>62</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>54</v>
       </c>
       <c r="E19" s="9">
         <v>2</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G19" s="12">
         <v>0.1</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I19" s="13">
         <v>415</v>
@@ -3482,30 +3339,30 @@
         <v>LS</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="28" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>121</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="59" t="s">
-        <v>56</v>
+        <v>63</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="E20" s="9">
         <v>2</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G20" s="18">
         <v>37</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I20" s="13">
         <v>415</v>
@@ -3532,30 +3389,30 @@
         <v>HP</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="28" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
         <v>121</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="59" t="s">
-        <v>57</v>
+        <v>64</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>56</v>
       </c>
       <c r="E21" s="9">
         <v>2</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G21" s="18">
         <v>37</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I21" s="13">
         <v>415</v>
@@ -3582,30 +3439,30 @@
         <v>HP</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="28" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <v>121</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="59" t="s">
-        <v>58</v>
+      <c r="D22" s="19" t="s">
+        <v>57</v>
       </c>
       <c r="E22" s="9">
         <v>2</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G22" s="18">
         <v>37</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I22" s="13">
         <v>415</v>
@@ -3632,30 +3489,30 @@
         <v>HP</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="28" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
         <v>121</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="59" t="s">
-        <v>59</v>
+      <c r="D23" s="19" t="s">
+        <v>58</v>
       </c>
       <c r="E23" s="9">
         <v>2</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G23" s="18">
         <v>37</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I23" s="13">
         <v>415</v>
@@ -3682,30 +3539,30 @@
         <v>HP</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="28" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
         <v>121</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="59" t="s">
-        <v>60</v>
+      <c r="D24" s="19" t="s">
+        <v>59</v>
       </c>
       <c r="E24" s="9">
         <v>2</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G24" s="18">
         <v>37</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I24" s="13">
         <v>415</v>
@@ -3732,30 +3589,30 @@
         <v>HP</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="28" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <v>121</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="59" t="s">
-        <v>61</v>
+        <v>65</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>60</v>
       </c>
       <c r="E25" s="9">
         <v>2</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G25" s="18">
         <v>37</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I25" s="13">
         <v>415</v>
@@ -3782,30 +3639,30 @@
         <v>HP</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="28" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <v>121</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D26" s="59" t="s">
-        <v>62</v>
+      <c r="D26" s="19" t="s">
+        <v>61</v>
       </c>
       <c r="E26" s="9">
         <v>2</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G26" s="18">
         <v>37</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I26" s="13">
         <v>415</v>
@@ -3853,24 +3710,24 @@
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="D7">
-    <cfRule type="duplicateValues" dxfId="20" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7">
-    <cfRule type="duplicateValues" dxfId="19" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7">
-    <cfRule type="duplicateValues" dxfId="18" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N7">
-    <cfRule type="duplicateValues" dxfId="17" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8:N26">
-    <cfRule type="expression" dxfId="16" priority="22">
+    <cfRule type="expression" dxfId="2" priority="22">
       <formula>ISERROR($O8)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8:O26">
-    <cfRule type="expression" dxfId="15" priority="21">
+    <cfRule type="expression" dxfId="1" priority="21">
       <formula>ISNA($O8)=TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>